<commit_message>
Buổi 11: nested router + layout
</commit_message>
<xml_diff>
--- a/diem_danh_giay_15_03_23_11_16_50.xlsx
+++ b/diem_danh_giay_15_03_23_11_16_50.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="16400"/>
+    <workbookView windowHeight="18800"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -422,8 +422,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -455,14 +455,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -476,9 +477,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -495,6 +495,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -509,7 +517,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -517,14 +546,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,45 +582,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -600,6 +593,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -620,7 +620,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,13 +650,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,25 +692,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,49 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,25 +746,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,31 +764,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,11 +823,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -843,24 +882,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,6 +903,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -890,181 +920,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1483,8 +1483,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1664,7 +1664,9 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1702,7 +1704,9 @@
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>9</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1740,7 +1744,9 @@
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>9</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1778,7 +1784,9 @@
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>9</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1816,7 +1824,9 @@
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1854,7 +1864,9 @@
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1892,7 +1904,9 @@
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1">
+        <v>9</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1930,7 +1944,9 @@
       <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>9</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1968,7 +1984,9 @@
       <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1">
+        <v>9</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2006,7 +2024,9 @@
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>9</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2044,7 +2064,9 @@
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1">
+        <v>9</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2082,7 +2104,9 @@
       <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1">
+        <v>9</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2118,7 +2142,9 @@
         <v>45</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2156,7 +2182,9 @@
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1">
+        <v>9</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2194,7 +2222,9 @@
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1">
+        <v>9</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2232,7 +2262,9 @@
       <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1">
+        <v>9</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2270,7 +2302,9 @@
       <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1">
+        <v>9</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2306,7 +2340,9 @@
         <v>60</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1">
+        <v>9</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2344,7 +2380,9 @@
       <c r="E24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1">
+        <v>9</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2382,7 +2420,9 @@
       <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1">
+        <v>9</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2420,7 +2460,9 @@
       <c r="E26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1">
+        <v>9</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2456,7 +2498,9 @@
         <v>72</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1">
+        <v>4</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2494,7 +2538,9 @@
       <c r="E28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1">
+        <v>9</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2532,7 +2578,9 @@
       <c r="E29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1">
+        <v>9</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2570,7 +2618,9 @@
       <c r="E30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1">
+        <v>9</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2608,7 +2658,9 @@
       <c r="E31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1">
+        <v>9</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2646,7 +2698,9 @@
       <c r="E32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1">
+        <v>9</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2684,7 +2738,9 @@
       <c r="E33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="1">
+        <v>4</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2722,7 +2778,9 @@
       <c r="E34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1">
+        <v>9</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2760,7 +2818,9 @@
       <c r="E35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1">
+        <v>9</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2798,7 +2858,9 @@
       <c r="E36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="1">
+        <v>9</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2836,7 +2898,9 @@
       <c r="E37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="1">
+        <v>9</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -2874,7 +2938,9 @@
       <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="1">
+        <v>9</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2912,7 +2978,9 @@
       <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="1"/>
+      <c r="F39" s="1">
+        <v>4</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2950,7 +3018,9 @@
       <c r="E40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1">
+        <v>9</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2988,7 +3058,9 @@
       <c r="E41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1">
+        <v>9</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -3026,7 +3098,9 @@
       <c r="E42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1">
+        <v>9</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -3064,7 +3138,9 @@
       <c r="E43" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1">
+        <v>9</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3102,7 +3178,9 @@
       <c r="E44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1">
+        <v>9</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>

</xml_diff>